<commit_message>
Completed final touch-ups and added updated form definition
</commit_message>
<xml_diff>
--- a/extras/test-form/Extra buttons.xlsx
+++ b/extras/test-form/Extra buttons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9E11F6-5E4A-9946-951C-899A584552C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027E0D53-8972-774B-88BC-18BF0BEEC9E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="393">
   <si>
     <t>type</t>
   </si>
@@ -2621,9 +2621,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Hey, this is required!</t>
-  </si>
-  <si>
     <t>What is your name?</t>
   </si>
   <si>
@@ -2633,11 +2630,6 @@
     <t>disp</t>
   </si>
   <si>
-    <t>${name}&lt;br&gt;
-${age}&lt;br&gt;
-${height}</t>
-  </si>
-  <si>
     <t>Please round to up to two decimal places!</t>
   </si>
   <si>
@@ -2650,124 +2642,30 @@
     <t>Please enter a number greater than 0.</t>
   </si>
   <si>
-    <t>custom-extrabuttons(A="Refused", B=-88)</t>
-  </si>
-  <si>
     <t>(.&gt;0 or .=-77 or .=-99 or .=-66 or .=-55) and int(. * 100) = .*100</t>
   </si>
   <si>
-    <t>custom-extrabuttons(A="I don't know", B=-99, C="I don't understand the question", D=-77, E="Who are you? How did I get here?", F=-66, G="Qu'est-ce que vous avez dit?", H=-55)</t>
-  </si>
-  <si>
     <t>Do not read the buttons aloud. Only select one if the respondent insists.</t>
   </si>
   <si>
     <t>Enter your height:</t>
   </si>
   <si>
-    <t>label:हिंदी</t>
-  </si>
-  <si>
-    <t>image:हिंदी</t>
-  </si>
-  <si>
-    <t>audio:हिंदी</t>
-  </si>
-  <si>
-    <t>video:हिंदी</t>
-  </si>
-  <si>
-    <t>label:português</t>
-  </si>
-  <si>
-    <t>image:português</t>
-  </si>
-  <si>
-    <t>audio:português</t>
-  </si>
-  <si>
-    <t>video:português</t>
-  </si>
-  <si>
-    <t>label:spanish</t>
-  </si>
-  <si>
-    <t>image:spanish</t>
-  </si>
-  <si>
-    <t>audio:spanish</t>
-  </si>
-  <si>
-    <t>video:spanish</t>
-  </si>
-  <si>
-    <t>hint:हिंदी</t>
-  </si>
-  <si>
-    <t>constraint message:हिंदी</t>
-  </si>
-  <si>
-    <t>required message:हिंदी</t>
-  </si>
-  <si>
-    <t>media:image:हिंदी</t>
-  </si>
-  <si>
-    <t>media:audio:हिंदी</t>
-  </si>
-  <si>
-    <t>media:video:हिंदी</t>
-  </si>
-  <si>
-    <t>hint:português</t>
-  </si>
-  <si>
-    <t>constraint message:português</t>
-  </si>
-  <si>
-    <t>required message:português</t>
-  </si>
-  <si>
-    <t>media:image:português</t>
-  </si>
-  <si>
-    <t>media:audio:português</t>
-  </si>
-  <si>
-    <t>media:video:português</t>
-  </si>
-  <si>
-    <t>hint:spanish</t>
-  </si>
-  <si>
-    <t>constraint message:spanish</t>
-  </si>
-  <si>
-    <t>required message:spanish</t>
-  </si>
-  <si>
-    <t>media:image:spanish</t>
-  </si>
-  <si>
-    <t>media:audio:spanish</t>
-  </si>
-  <si>
-    <t>media:video:spanish</t>
-  </si>
-  <si>
-    <t>तुम्हारा नाम क्या हे?</t>
-  </si>
-  <si>
-    <t>Qual é o seu nome?</t>
-  </si>
-  <si>
-    <t>¿Cuál es tu nombre?</t>
-  </si>
-  <si>
-    <t>custom-extrabuttons(A="I don't know", B=-99, C="Refused", D=-88, E="I don't understand the question", F=-77)</t>
-  </si>
-  <si>
     <t>.&gt;=0 or  .= -77 or .=-88 or .=-99</t>
+  </si>
+  <si>
+    <t>custom-extrabuttons(message=1, yes=1, no=1, button='Refused', value=-88)</t>
+  </si>
+  <si>
+    <t>custom-extrabuttons(message=1, yes=1, no='Nope', button1="I don't know", value1=-99, button2="I don't understand the question", value2=-77, button3="Who are you? How did I get here?", value3=-66, button4="Qu'est-ce que vous avez dit?", value4=-55)</t>
+  </si>
+  <si>
+    <t>custom-extrabuttons(message='Voulez-vous vraiment remplacer "oldValue" par "replacementValue"?', yes='Oui', no='Non', button1="I don't know", value1=-99, button2='Refused', value2=-88, button3="I don't understand the question", value3=-77))</t>
+  </si>
+  <si>
+    <t>Name: ${name}&lt;br&gt;
+Age: ${age}&lt;br&gt;
+Height: ${height}</t>
   </si>
 </sst>
 </file>
@@ -3216,7 +3114,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3364,6 +3262,13 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="108">
@@ -4917,11 +4822,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR14"/>
+  <dimension ref="A1:AR15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5022,67 +4927,67 @@
         <v>286</v>
       </c>
       <c r="X1" t="s">
-        <v>392</v>
+        <v>358</v>
       </c>
       <c r="Y1" t="s">
-        <v>404</v>
+        <v>358</v>
       </c>
       <c r="Z1" t="s">
-        <v>405</v>
+        <v>358</v>
       </c>
       <c r="AA1" t="s">
-        <v>406</v>
+        <v>358</v>
       </c>
       <c r="AB1" t="s">
-        <v>407</v>
+        <v>358</v>
       </c>
       <c r="AC1" t="s">
-        <v>408</v>
+        <v>358</v>
       </c>
       <c r="AD1" t="s">
-        <v>409</v>
+        <v>358</v>
       </c>
       <c r="AE1" t="s">
-        <v>396</v>
+        <v>358</v>
       </c>
       <c r="AF1" t="s">
-        <v>410</v>
+        <v>358</v>
       </c>
       <c r="AG1" t="s">
-        <v>411</v>
+        <v>358</v>
       </c>
       <c r="AH1" t="s">
-        <v>412</v>
+        <v>358</v>
       </c>
       <c r="AI1" t="s">
-        <v>413</v>
+        <v>358</v>
       </c>
       <c r="AJ1" t="s">
-        <v>414</v>
+        <v>358</v>
       </c>
       <c r="AK1" t="s">
-        <v>415</v>
+        <v>358</v>
       </c>
       <c r="AL1" t="s">
-        <v>400</v>
+        <v>358</v>
       </c>
       <c r="AM1" t="s">
-        <v>416</v>
+        <v>358</v>
       </c>
       <c r="AN1" t="s">
-        <v>417</v>
+        <v>358</v>
       </c>
       <c r="AO1" t="s">
-        <v>418</v>
+        <v>358</v>
       </c>
       <c r="AP1" t="s">
-        <v>419</v>
+        <v>358</v>
       </c>
       <c r="AQ1" t="s">
-        <v>420</v>
+        <v>358</v>
       </c>
       <c r="AR1" t="s">
-        <v>421</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:44" ht="17" x14ac:dyDescent="0.2">
@@ -5235,71 +5140,41 @@
         <v>373</v>
       </c>
     </row>
-    <row r="11" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+      <c r="A11" s="64"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="66"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="V11"/>
+    </row>
+    <row r="12" spans="1:44" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>87</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C11" t="s">
-        <v>379</v>
-      </c>
-      <c r="D11" t="s">
-        <v>390</v>
-      </c>
-      <c r="F11" t="s">
-        <v>387</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="C12" t="s">
+        <v>378</v>
+      </c>
+      <c r="D12" t="s">
+        <v>386</v>
+      </c>
+      <c r="F12" t="s">
+        <v>389</v>
+      </c>
+      <c r="G12" t="s">
         <v>358</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>358</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>358</v>
-      </c>
-      <c r="K11" t="s">
-        <v>377</v>
-      </c>
-      <c r="L11" t="s">
-        <v>358</v>
-      </c>
-      <c r="X11" t="s">
-        <v>422</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>423</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="12" spans="1:44" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="D12" t="s">
-        <v>390</v>
-      </c>
-      <c r="F12" t="s">
-        <v>425</v>
-      </c>
-      <c r="G12" t="s">
-        <v>426</v>
-      </c>
-      <c r="H12" t="s">
-        <v>386</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>358</v>
@@ -5311,46 +5186,88 @@
         <v>377</v>
       </c>
       <c r="L12" t="s">
-        <v>378</v>
+        <v>358</v>
+      </c>
+      <c r="X12" t="s">
+        <v>358</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>358</v>
+      </c>
+      <c r="AL12" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="13" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="D13" t="s">
+        <v>386</v>
+      </c>
+      <c r="F13" t="s">
         <v>391</v>
-      </c>
-      <c r="D13" t="s">
-        <v>390</v>
-      </c>
-      <c r="F13" t="s">
-        <v>389</v>
       </c>
       <c r="G13" t="s">
         <v>388</v>
       </c>
       <c r="H13" t="s">
-        <v>383</v>
+        <v>384</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>358</v>
       </c>
       <c r="K13" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="14" spans="1:44" ht="51" x14ac:dyDescent="0.2">
+      <c r="L13"/>
+    </row>
+    <row r="14" spans="1:44" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="D14" t="s">
+        <v>386</v>
+      </c>
+      <c r="F14" t="s">
+        <v>390</v>
+      </c>
+      <c r="G14" t="s">
+        <v>385</v>
+      </c>
+      <c r="H14" t="s">
+        <v>381</v>
+      </c>
+      <c r="K14" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="B15" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="K15" t="s">
         <v>373</v>
       </c>
     </row>
@@ -5533,40 +5450,40 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>392</v>
+        <v>358</v>
       </c>
       <c r="G1" t="s">
-        <v>393</v>
+        <v>358</v>
       </c>
       <c r="H1" t="s">
-        <v>394</v>
+        <v>358</v>
       </c>
       <c r="I1" t="s">
-        <v>395</v>
+        <v>358</v>
       </c>
       <c r="J1" t="s">
-        <v>396</v>
+        <v>358</v>
       </c>
       <c r="K1" t="s">
-        <v>397</v>
+        <v>358</v>
       </c>
       <c r="L1" t="s">
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="M1" t="s">
-        <v>399</v>
+        <v>358</v>
       </c>
       <c r="N1" t="s">
-        <v>400</v>
+        <v>358</v>
       </c>
       <c r="O1" t="s">
-        <v>401</v>
+        <v>358</v>
       </c>
       <c r="P1" t="s">
-        <v>402</v>
+        <v>358</v>
       </c>
       <c r="Q1" t="s">
-        <v>403</v>
+        <v>358</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -5680,14 +5597,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2002261819</v>
+        <v>2002281906</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
Updated form definition spreadsheet with Arabic example
</commit_message>
<xml_diff>
--- a/extras/test-form/Extra buttons.xlsx
+++ b/extras/test-form/Extra buttons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/extra-buttons/extras/test-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027E0D53-8972-774B-88BC-18BF0BEEC9E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A4F7E1-8F79-604C-9066-BBE006647379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24280" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="396">
   <si>
     <t>type</t>
   </si>
@@ -2616,9 +2616,6 @@
   </si>
   <si>
     <t>How old are you?</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
   <si>
     <t>What is your name?</t>
@@ -2666,6 +2663,18 @@
     <t>Name: ${name}&lt;br&gt;
 Age: ${age}&lt;br&gt;
 Height: ${height}</t>
+  </si>
+  <si>
+    <t>arabic_example</t>
+  </si>
+  <si>
+    <t>custom-extrabuttons(message='هل أنت متأكد من أنك تريد استبدال القيمة؟', yes='نعم', no='لا', button='رفض', value=-88)</t>
+  </si>
+  <si>
+    <t>ما اسمك؟</t>
+  </si>
+  <si>
+    <t>لا تقرأ الأزرار بصوت عالٍ. حدد واحدًا فقط إذا أصر المستجيب.</t>
   </si>
 </sst>
 </file>
@@ -3230,6 +3239,13 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3262,13 +3278,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="108">
@@ -4822,11 +4831,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR15"/>
+  <dimension ref="A1:AR16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5141,17 +5150,17 @@
       </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="A11" s="64"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="66"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="55"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
       <c r="V11"/>
     </row>
     <row r="12" spans="1:44" ht="17" x14ac:dyDescent="0.2">
@@ -5162,13 +5171,13 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G12" t="s">
         <v>358</v>
@@ -5182,9 +5191,7 @@
       <c r="J12" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="K12" t="s">
-        <v>377</v>
-      </c>
+      <c r="K12"/>
       <c r="L12" t="s">
         <v>358</v>
       </c>
@@ -5209,16 +5216,16 @@
         <v>376</v>
       </c>
       <c r="D13" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F13" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>358</v>
@@ -5226,9 +5233,7 @@
       <c r="J13" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="K13" t="s">
-        <v>377</v>
-      </c>
+      <c r="K13"/>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:44" ht="17" x14ac:dyDescent="0.2">
@@ -5236,39 +5241,54 @@
         <v>92</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H14" t="s">
-        <v>381</v>
-      </c>
-      <c r="K14" t="s">
-        <v>377</v>
-      </c>
+        <v>380</v>
+      </c>
+      <c r="K14"/>
     </row>
     <row r="15" spans="1:44" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K15" t="s">
         <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -5597,14 +5617,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>382</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>383</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2002281906</v>
+        <v>2005121839</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>
@@ -5639,22 +5659,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="61"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -5848,10 +5868,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="62" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -8641,10 +8661,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="63" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="61"/>
+      <c r="B83" s="64"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -9804,20 +9824,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="57"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="61"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -9892,28 +9912,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="66"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="59"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="61"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>